<commit_message>
final del proyecto en su primera version
</commit_message>
<xml_diff>
--- a/Datos futplay.xlsx
+++ b/Datos futplay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaqu\Ficha Medica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B23E0AB-4600-4A29-BD30-8481062B23B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E474051-79EC-46FD-92B9-873BC1444EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -857,9 +857,6 @@
     <t>Single Leg Squad 1</t>
   </si>
   <si>
-    <t>Sinlge Leg Squad2</t>
-  </si>
-  <si>
     <t>Salto1</t>
   </si>
   <si>
@@ -960,6 +957,9 @@
   </si>
   <si>
     <t>Quilpue</t>
+  </si>
+  <si>
+    <t>SingLe Leg Squad2</t>
   </si>
 </sst>
 </file>
@@ -1431,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG978"/>
+  <dimension ref="A1:AF978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1467,7 +1467,7 @@
     <col min="31" max="32" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1477,95 +1477,95 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="AC1" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE1" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="F1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AB1" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="AD1" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="AE1" s="25" t="s">
-        <v>274</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>306</v>
-      </c>
     </row>
-    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -1575,95 +1575,95 @@
       <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="7">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="7">
+        <v>83</v>
+      </c>
+      <c r="S2" s="7">
+        <v>98</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="7">
+        <v>29</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="AD2" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="AE2" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="AF2" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="G2" s="7">
-        <v>85</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="7">
-        <v>83</v>
-      </c>
-      <c r="J2" s="7">
-        <v>98</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="7">
-        <v>29</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="AC2" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="3" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
@@ -1673,95 +1673,95 @@
       <c r="C3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="7">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="7">
+        <v>71</v>
+      </c>
+      <c r="S3" s="7">
+        <v>99</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AD3" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="G3" s="7">
-        <v>70</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="7">
-        <v>71</v>
-      </c>
-      <c r="J3" s="7">
-        <v>99</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC3" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="AD3" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="AE3" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AF3" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="4" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
@@ -1769,87 +1769,87 @@
         <v>36</v>
       </c>
       <c r="C4" s="14"/>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="7">
+        <v>88</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="7">
+        <v>76</v>
+      </c>
+      <c r="S4" s="7">
+        <v>99</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AD4" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="AE4" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="AF4" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="G4" s="7">
-        <v>88</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="7">
-        <v>76</v>
-      </c>
-      <c r="J4" s="7">
-        <v>99</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="S4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="AC4" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD4" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AE4" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AF4" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="5" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>61</v>
       </c>
@@ -1857,87 +1857,87 @@
         <v>39</v>
       </c>
       <c r="C5" s="14"/>
-      <c r="D5" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="D5" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="7">
         <v>98</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="15">
+      <c r="R5" s="15">
         <v>86</v>
       </c>
-      <c r="J5" s="15">
+      <c r="S5" s="15">
         <v>99</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="T5" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="U5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="V5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="W5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="X5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="Y5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
+      <c r="Z5" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="AA5" s="13" t="s">
+        <v>280</v>
+      </c>
       <c r="AB5" s="13" t="s">
         <v>280</v>
       </c>
       <c r="AC5" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD5" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AE5" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="AF5" s="12" t="s">
-        <v>307</v>
+        <v>288</v>
+      </c>
+      <c r="AD5" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE5" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="AF5" s="14" t="s">
+        <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>71</v>
       </c>
@@ -1947,87 +1947,87 @@
       <c r="C6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="7">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="7">
+        <v>22</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA6" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB6" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD6" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="AE6" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="AF6" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G6" s="7">
-        <v>61</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="7">
-        <v>22</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W6" s="14"/>
-      <c r="X6" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB6" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC6" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="AD6" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="AE6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF6" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="7" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>80</v>
       </c>
@@ -2037,87 +2037,87 @@
       <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="7">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB7" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC7" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD7" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="AE7" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="7">
-        <v>100</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y7" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB7" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AC7" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD7" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="AE7" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="AF7" s="12" t="s">
-        <v>307</v>
-      </c>
+      <c r="AF7" s="8"/>
     </row>
-    <row r="8" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>88</v>
       </c>
@@ -2127,85 +2127,85 @@
       <c r="C8" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="7">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="X8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA8" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB8" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AC8" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="AD8" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="AE8" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="AF8" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="G8" s="7">
-        <v>85</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="T8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="V8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W8" s="14"/>
-      <c r="X8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y8" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z8" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC8" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD8" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AE8" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF8" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="9" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>97</v>
       </c>
@@ -2215,87 +2215,87 @@
       <c r="C9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="7">
+        <v>86</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA9" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB9" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AC9" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="AD9" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="AE9" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="AF9" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="G9" s="7">
-        <v>86</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="W9" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="X9" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB9" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC9" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AD9" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AE9" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="AF9" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="10" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>105</v>
       </c>
@@ -2305,90 +2305,89 @@
       <c r="C10" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="7">
+        <v>91</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z10" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA10" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB10" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC10" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD10" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="AE10" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="AF10" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G10" s="7">
-        <v>91</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S10" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X10" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y10" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB10" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC10" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AD10" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE10" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF10" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="AG10" s="21"/>
     </row>
-    <row r="11" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -2398,87 +2397,87 @@
       <c r="C11" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="7">
+        <v>84</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA11" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB11" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="AC11" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="AD11" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="AE11" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="AF11" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="7">
-        <v>84</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S11" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="T11" s="14"/>
-      <c r="U11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="V11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="W11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y11" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z11" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB11" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC11" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AD11" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="AE11" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="AF11" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="12" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>122</v>
       </c>
@@ -2488,89 +2487,89 @@
       <c r="C12" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="P12" s="7">
+        <v>75</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA12" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB12" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC12" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="AD12" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="AE12" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="AF12" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="G12" s="7">
-        <v>75</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="T12" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="V12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X12" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y12" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z12" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA12" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB12" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC12" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD12" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AE12" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="AF12" s="12" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="13" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>135</v>
       </c>
@@ -2578,95 +2577,95 @@
         <v>35</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="D13" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="7">
         <v>98</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="Q13" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="I13" s="7">
+      <c r="R13" s="7">
         <v>50</v>
       </c>
-      <c r="J13" s="7">
+      <c r="S13" s="7">
         <v>99</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="T13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="U13" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="V13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="W13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="X13" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="Y13" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="Q13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="T13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y13" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA13" s="27" t="s">
-        <v>33</v>
+      <c r="Z13" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA13" s="17" t="s">
+        <v>285</v>
       </c>
       <c r="AB13" s="17" t="s">
         <v>282</v>
       </c>
       <c r="AC13" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="AD13" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="AE13" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="AF13" s="12" t="s">
-        <v>307</v>
+        <v>282</v>
+      </c>
+      <c r="AD13" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE13" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF13" s="16" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>142</v>
       </c>
@@ -2674,95 +2673,95 @@
         <v>37</v>
       </c>
       <c r="C14" s="16"/>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="P14" s="7">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="R14" s="7">
+        <v>98</v>
+      </c>
+      <c r="S14" s="7">
+        <v>98</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W14" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA14" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB14" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="AC14" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="AD14" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE14" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="AF14" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="G14" s="7">
-        <v>114</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="7">
-        <v>98</v>
-      </c>
-      <c r="J14" s="7">
-        <v>98</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X14" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA14" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB14" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="AC14" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD14" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="AE14" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="AF14" s="12" t="s">
-        <v>308</v>
-      </c>
     </row>
-    <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>150</v>
       </c>
@@ -2772,95 +2771,95 @@
       <c r="C15" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15" s="7">
+        <v>81</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" s="7">
+        <v>77</v>
+      </c>
+      <c r="S15" s="7">
+        <v>99</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA15" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="AB15" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="AC15" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="AD15" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="AE15" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="AF15" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="G15" s="7">
-        <v>81</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="7">
-        <v>77</v>
-      </c>
-      <c r="J15" s="7">
-        <v>99</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W15" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="X15" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y15" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB15" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="AC15" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="AD15" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="AE15" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF15" s="12" t="s">
-        <v>308</v>
-      </c>
     </row>
-    <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>156</v>
       </c>
@@ -2870,92 +2869,92 @@
       <c r="C16" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="7">
+        <v>81</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R16" s="7">
+        <v>70</v>
+      </c>
+      <c r="S16" s="7">
+        <v>98</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="V16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="AA16" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB16" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="AC16" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="AD16" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="AE16" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="AF16" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="G16" s="7">
-        <v>81</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="7">
-        <v>70</v>
-      </c>
-      <c r="J16" s="7">
-        <v>98</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S16" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="T16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="V16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W16" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="X16" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y16" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB16" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="AC16" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD16" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE16" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="AF16" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2968,92 +2967,92 @@
       <c r="C17" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="P17" s="7">
+        <v>91</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R17" s="7">
+        <v>65</v>
+      </c>
+      <c r="S17" s="7">
+        <v>99</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="X17" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z17" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA17" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB17" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="AC17" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD17" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="AE17" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="AF17" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="G17" s="7">
-        <v>91</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17" s="7">
-        <v>65</v>
-      </c>
-      <c r="J17" s="7">
-        <v>99</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O17" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R17" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="S17" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="T17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U17" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="V17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X17" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y17" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA17" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="AB17" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="AC17" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD17" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="AE17" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="AF17" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3064,92 +3063,92 @@
         <v>34</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="7">
+        <v>115</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="R18" s="7">
+        <v>81</v>
+      </c>
+      <c r="S18" s="7">
+        <v>98</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="V18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W18" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="X18" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA18" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="AB18" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="AC18" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD18" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="AE18" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="AF18" s="16" t="s">
         <v>257</v>
-      </c>
-      <c r="G18" s="7">
-        <v>115</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="I18" s="7">
-        <v>81</v>
-      </c>
-      <c r="J18" s="7">
-        <v>98</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="O18" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="P18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R18" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S18" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="T18" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="U18" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="V18" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="W18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X18" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y18" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB18" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC18" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="AD18" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="AE18" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="AF18" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3162,92 +3161,92 @@
       <c r="C19" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="P19" s="7">
+        <v>96</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="R19" s="7">
+        <v>68</v>
+      </c>
+      <c r="S19" s="7">
+        <v>97</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z19" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA19" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB19" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC19" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AD19" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="AE19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="AF19" s="7" t="s">
         <v>259</v>
-      </c>
-      <c r="G19" s="7">
-        <v>96</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="I19" s="7">
-        <v>68</v>
-      </c>
-      <c r="J19" s="7">
-        <v>97</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S19" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X19" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y19" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z19" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA19" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB19" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC19" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="AD19" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="AE19" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="AF19" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3260,92 +3259,92 @@
       <c r="C20" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="7">
+        <v>90</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="R20" s="7">
+        <v>62</v>
+      </c>
+      <c r="S20" s="7">
+        <v>99</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="V20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W20" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="X20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z20" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA20" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="AB20" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC20" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="AD20" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="AE20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="AF20" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="G20" s="7">
-        <v>90</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20" s="7">
-        <v>62</v>
-      </c>
-      <c r="J20" s="7">
-        <v>99</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="O20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="P20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q20" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S20" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U20" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="V20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y20" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="Z20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB20" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC20" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="AD20" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="AE20" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="AF20" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3358,92 +3357,92 @@
       <c r="C21" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="P21" s="7">
+        <v>85</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="R21" s="7">
+        <v>66</v>
+      </c>
+      <c r="S21" s="7">
+        <v>97</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W21" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="X21" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA21" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB21" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC21" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD21" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="AE21" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="AF21" s="26" t="s">
         <v>264</v>
-      </c>
-      <c r="G21" s="7">
-        <v>85</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="I21" s="7">
-        <v>66</v>
-      </c>
-      <c r="J21" s="7">
-        <v>97</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="P21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q21" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S21" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="T21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U21" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="V21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="X21" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y21" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z21" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA21" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="AB21" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="AC21" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="AD21" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="AE21" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="AF21" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3456,111 +3455,108 @@
       <c r="C22" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="P22" s="7">
+        <v>119</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="R22" s="7">
+        <v>82</v>
+      </c>
+      <c r="S22" s="7">
+        <v>99</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W22" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="X22" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z22" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA22" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB22" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC22" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="AD22" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="AE22" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="AF22" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="G22" s="7">
-        <v>119</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I22" s="7">
-        <v>82</v>
-      </c>
-      <c r="J22" s="7">
-        <v>99</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S22" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="T22" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="U22" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="V22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="W22" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="X22" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="Y22" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA22" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB22" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="AC22" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD22" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="AE22" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="AF22" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AF23" s="28"/>
+      <c r="D23" s="28"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="19"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AA26" s="21"/>
     </row>
     <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="19"/>
-    </row>
+    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>